<commit_message>
add decimal place info for floats on reading from sheet
</commit_message>
<xml_diff>
--- a/spec/support/static_test_files/cell_values_and_formats.xlsx
+++ b/spec/support/static_test_files/cell_values_and_formats.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/f3m-mbp1/dev/f3mmedia/rxl/spec/support/static_test_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B516D5ED-AD5A-064D-A3A7-05596DF69732}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="0" windowWidth="25600" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="25600" windowHeight="16100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="string" sheetId="2" r:id="rId1"/>
     <sheet name="number" sheetId="3" r:id="rId2"/>
     <sheet name="float" sheetId="4" r:id="rId3"/>
-    <sheet name="date" sheetId="5" r:id="rId4"/>
-    <sheet name="time" sheetId="6" r:id="rId5"/>
-    <sheet name="percentage" sheetId="7" r:id="rId6"/>
-    <sheet name="percentage_float" sheetId="9" r:id="rId7"/>
-    <sheet name="empty" sheetId="8" r:id="rId8"/>
+    <sheet name="zero_float" sheetId="10" r:id="rId4"/>
+    <sheet name="date" sheetId="5" r:id="rId5"/>
+    <sheet name="time" sheetId="6" r:id="rId6"/>
+    <sheet name="percentage" sheetId="7" r:id="rId7"/>
+    <sheet name="percentage_float" sheetId="9" r:id="rId8"/>
+    <sheet name="empty" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="35">
   <si>
     <t>number</t>
   </si>
@@ -125,14 +132,20 @@
   </si>
   <si>
     <t>=50%+50%</t>
+  </si>
+  <si>
+    <t>123.00</t>
+  </si>
+  <si>
+    <t>=122.41+0.59</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -389,6 +402,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -713,20 +734,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -734,7 +755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -746,7 +767,7 @@
         <v>abcde</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -758,7 +779,7 @@
         <v>abcde</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -770,7 +791,7 @@
         <v>abcde</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -782,7 +803,7 @@
         <v>abcde</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -794,7 +815,7 @@
         <v>abcde</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -818,20 +839,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -839,7 +860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -851,7 +872,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -862,7 +883,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -874,7 +895,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -885,7 +906,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -896,7 +917,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -919,20 +940,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -940,7 +961,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -951,7 +972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -962,7 +983,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -974,7 +995,7 @@
         <v>123.45</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -986,7 +1007,7 @@
         <v>1000000000.4499999</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -998,7 +1019,7 @@
         <v>999999999.44999993</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1020,20 +1041,116 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA70A8D-D14F-4646-B304-AA201E8A5DD4}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="3" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>123</v>
+      </c>
+      <c r="C4" s="3">
+        <f>122.41+0.59</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1000000000.12</v>
+      </c>
+      <c r="C5" s="1">
+        <f>999999999.41+1.04</f>
+        <v>1000000000.4499999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1000000000.12</v>
+      </c>
+      <c r="C6" s="8">
+        <f>999999999.41+0.04</f>
+        <v>999999999.44999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1041,7 +1158,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1052,7 +1169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1063,7 +1180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1074,7 +1191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1086,7 +1203,7 @@
         <v>36526</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1098,7 +1215,7 @@
         <v>36526</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1107,105 +1224,6 @@
       </c>
       <c r="C7" s="6" t="s">
         <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="3" width="35.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.42743055555555554</v>
-      </c>
-      <c r="C6" s="8">
-        <f>TIME(10,15,30)</f>
-        <v>0.42743055555555554</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1219,20 +1237,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1240,29 +1258,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1273,38 +1291,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="B6" s="8">
+        <v>0.42743055555555554</v>
+      </c>
+      <c r="C6" s="8">
+        <f>TIME(10,15,30)</f>
+        <v>0.42743055555555554</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <f>50%+50%</f>
-        <v>1</v>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1318,20 +1336,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1339,7 +1357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1350,18 +1368,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1383,7 +1401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1394,16 +1412,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6">
-        <v>1.2344999999999999</v>
-      </c>
-      <c r="C7" s="6">
-        <f>123.41%+0.04%</f>
-        <v>1.2344999999999999</v>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <f>50%+50%</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1417,20 +1435,119 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="3" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1.2344999999999999</v>
+      </c>
+      <c r="C7" s="6">
+        <f>123.41%+0.04%</f>
+        <v>1.2344999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1438,7 +1555,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1446,7 +1563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1455,7 +1572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1473,7 +1590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1482,7 +1599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
updates and tests for output format, cell formatting and formulas (#6)
* update readme and version

* add write file as tables functionality

* add rxl gem versions to gitignore

* set rubyXL version to 3.3.30 due to center alignment bug in 3.3.33

* add formatting for tables

* set rxl version to 0.4.0

* fix bug in formatting for nil cells, update tests to work for latest features

* increment version for bug fix

* add decimal place info for floats on reading from sheet

* refine cell format specification for write

* add formula tests for write

* add tests for cell formatting
</commit_message>
<xml_diff>
--- a/spec/support/static_test_files/cell_values_and_formats.xlsx
+++ b/spec/support/static_test_files/cell_values_and_formats.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/f3m-mbp1/dev/f3mmedia/rxl/spec/support/static_test_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B516D5ED-AD5A-064D-A3A7-05596DF69732}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="0" windowWidth="25600" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="25600" windowHeight="16100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="string" sheetId="2" r:id="rId1"/>
     <sheet name="number" sheetId="3" r:id="rId2"/>
     <sheet name="float" sheetId="4" r:id="rId3"/>
-    <sheet name="date" sheetId="5" r:id="rId4"/>
-    <sheet name="time" sheetId="6" r:id="rId5"/>
-    <sheet name="percentage" sheetId="7" r:id="rId6"/>
-    <sheet name="percentage_float" sheetId="9" r:id="rId7"/>
-    <sheet name="empty" sheetId="8" r:id="rId8"/>
+    <sheet name="zero_float" sheetId="10" r:id="rId4"/>
+    <sheet name="date" sheetId="5" r:id="rId5"/>
+    <sheet name="time" sheetId="6" r:id="rId6"/>
+    <sheet name="percentage" sheetId="7" r:id="rId7"/>
+    <sheet name="percentage_float" sheetId="9" r:id="rId8"/>
+    <sheet name="empty" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="35">
   <si>
     <t>number</t>
   </si>
@@ -125,14 +132,20 @@
   </si>
   <si>
     <t>=50%+50%</t>
+  </si>
+  <si>
+    <t>123.00</t>
+  </si>
+  <si>
+    <t>=122.41+0.59</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -389,6 +402,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -713,20 +734,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -734,7 +755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -746,7 +767,7 @@
         <v>abcde</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -758,7 +779,7 @@
         <v>abcde</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -770,7 +791,7 @@
         <v>abcde</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -782,7 +803,7 @@
         <v>abcde</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -794,7 +815,7 @@
         <v>abcde</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -818,20 +839,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -839,7 +860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -851,7 +872,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -862,7 +883,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -874,7 +895,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -885,7 +906,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -896,7 +917,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -919,20 +940,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -940,7 +961,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -951,7 +972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -962,7 +983,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -974,7 +995,7 @@
         <v>123.45</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -986,7 +1007,7 @@
         <v>1000000000.4499999</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -998,7 +1019,7 @@
         <v>999999999.44999993</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1020,20 +1041,116 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA70A8D-D14F-4646-B304-AA201E8A5DD4}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="3" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>123</v>
+      </c>
+      <c r="C4" s="3">
+        <f>122.41+0.59</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1000000000.12</v>
+      </c>
+      <c r="C5" s="1">
+        <f>999999999.41+1.04</f>
+        <v>1000000000.4499999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1000000000.12</v>
+      </c>
+      <c r="C6" s="8">
+        <f>999999999.41+0.04</f>
+        <v>999999999.44999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1041,7 +1158,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1052,7 +1169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1063,7 +1180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1074,7 +1191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1086,7 +1203,7 @@
         <v>36526</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1098,7 +1215,7 @@
         <v>36526</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1107,105 +1224,6 @@
       </c>
       <c r="C7" s="6" t="s">
         <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="3" width="35.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.42743055555555554</v>
-      </c>
-      <c r="C6" s="8">
-        <f>TIME(10,15,30)</f>
-        <v>0.42743055555555554</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1219,20 +1237,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1240,29 +1258,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1273,38 +1291,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="B6" s="8">
+        <v>0.42743055555555554</v>
+      </c>
+      <c r="C6" s="8">
+        <f>TIME(10,15,30)</f>
+        <v>0.42743055555555554</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <f>50%+50%</f>
-        <v>1</v>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1318,20 +1336,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1339,7 +1357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1350,18 +1368,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1383,7 +1401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1394,16 +1412,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6">
-        <v>1.2344999999999999</v>
-      </c>
-      <c r="C7" s="6">
-        <f>123.41%+0.04%</f>
-        <v>1.2344999999999999</v>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <f>50%+50%</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1417,20 +1435,119 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="3" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1.2344999999999999</v>
+      </c>
+      <c r="C7" s="6">
+        <f>123.41%+0.04%</f>
+        <v>1.2344999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
@@ -1438,7 +1555,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1446,7 +1563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1455,7 +1572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1473,7 +1590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1482,7 +1599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>

</xml_diff>